<commit_message>
MaJ de DdD et DF
</commit_message>
<xml_diff>
--- a/Analyse/Dictionnaire de données.xlsx
+++ b/Analyse/Dictionnaire de données.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taver\OneDrive\Documents\A1\PROJET\Projet 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MPN\Desktop\Prj BDD\GiselleMagicArts\Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -267,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -281,6 +281,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,17 +606,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -618,8 +627,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -629,8 +638,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
       <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
@@ -638,8 +647,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="14"/>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -647,8 +656,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -656,8 +665,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -665,8 +674,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -674,8 +683,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
       <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
@@ -683,8 +692,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
@@ -692,7 +701,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
       <c r="B10" s="7" t="s">
         <v>38</v>
       </c>
@@ -700,7 +710,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
       <c r="B11" s="7" t="s">
         <v>42</v>
       </c>
@@ -708,7 +719,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
       <c r="B12" s="7" t="s">
         <v>41</v>
       </c>
@@ -716,7 +728,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
       <c r="B13" s="7" t="s">
         <v>40</v>
       </c>
@@ -724,7 +737,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
       <c r="B14" s="7" t="s">
         <v>39</v>
       </c>
@@ -732,8 +746,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
       <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
@@ -741,8 +755,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
       <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
@@ -750,8 +764,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -761,8 +775,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
       <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
@@ -770,8 +784,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
         <v>3</v>
       </c>
@@ -779,8 +793,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="14"/>
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -788,8 +802,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
@@ -797,8 +811,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
       <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
@@ -806,8 +820,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
       <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
@@ -815,8 +829,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
       <c r="B24" s="1" t="s">
         <v>2</v>
       </c>
@@ -824,8 +838,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -835,8 +849,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
       <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
@@ -844,8 +858,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
       <c r="B27" s="3" t="s">
         <v>11</v>
       </c>
@@ -853,8 +867,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
       <c r="B28" s="1" t="s">
         <v>15</v>
       </c>
@@ -862,8 +876,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -873,8 +887,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="14"/>
       <c r="B30" s="3" t="s">
         <v>15</v>
       </c>
@@ -882,8 +896,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
@@ -891,8 +905,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="14"/>
       <c r="B32" s="3" t="s">
         <v>32</v>
       </c>
@@ -900,8 +914,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="14"/>
       <c r="B33" s="7" t="s">
         <v>35</v>
       </c>
@@ -909,8 +923,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="14"/>
       <c r="B34" s="7" t="s">
         <v>33</v>
       </c>
@@ -918,8 +932,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="15"/>
       <c r="B35" s="9" t="s">
         <v>34</v>
       </c>
@@ -927,8 +941,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -938,8 +952,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="14"/>
       <c r="B37" s="3" t="s">
         <v>22</v>
       </c>
@@ -947,8 +961,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="14"/>
       <c r="B38" s="3" t="s">
         <v>19</v>
       </c>
@@ -956,8 +970,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="14"/>
       <c r="B39" s="3" t="s">
         <v>29</v>
       </c>
@@ -965,8 +979,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="14"/>
       <c r="B40" s="3" t="s">
         <v>30</v>
       </c>
@@ -974,8 +988,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="14"/>
       <c r="B41" s="3" t="s">
         <v>6</v>
       </c>
@@ -983,8 +997,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="14"/>
       <c r="B42" s="3" t="s">
         <v>31</v>
       </c>
@@ -992,8 +1006,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="14"/>
       <c r="B43" s="7" t="s">
         <v>9</v>
       </c>
@@ -1001,8 +1015,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="14"/>
       <c r="B44" s="7" t="s">
         <v>32</v>
       </c>
@@ -1010,7 +1024,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="14"/>
       <c r="B45" s="7" t="s">
         <v>43</v>
       </c>
@@ -1018,7 +1033,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="14"/>
       <c r="B46" s="7" t="s">
         <v>51</v>
       </c>
@@ -1026,8 +1042,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="14"/>
       <c r="B47" s="7" t="s">
         <v>36</v>
       </c>
@@ -1035,8 +1051,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="15"/>
       <c r="B48" s="9" t="s">
         <v>37</v>
       </c>
@@ -1044,8 +1060,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B49" s="11" t="s">
@@ -1055,8 +1071,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="14"/>
       <c r="B50" s="7" t="s">
         <v>19</v>
       </c>
@@ -1064,8 +1080,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="14"/>
       <c r="B51" s="7" t="s">
         <v>2</v>
       </c>
@@ -1073,8 +1089,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="15"/>
       <c r="B52" s="9" t="s">
         <v>45</v>
       </c>
@@ -1082,8 +1098,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B53" s="11" t="s">
@@ -1093,8 +1109,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="14"/>
       <c r="B54" s="7" t="s">
         <v>48</v>
       </c>
@@ -1102,8 +1118,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="14"/>
       <c r="B55" s="7" t="s">
         <v>49</v>
       </c>
@@ -1111,8 +1127,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="15"/>
       <c r="B56" s="9" t="s">
         <v>52</v>
       </c>
@@ -1120,12 +1136,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A17:A24"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A36:A48"/>
+    <mergeCell ref="A49:A52"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>